<commit_message>
Finished! Everything works correctly now (I think)
The reset option for LZWmod works, there are no extra bytes
in the non reset version, the writeup has been corrected.
Everything should be good now!
</commit_message>
<xml_diff>
--- a/Assignment3/CompressionResults.xlsx
+++ b/Assignment3/CompressionResults.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewhrydil/Desktop/CurrentClassesLocal/CS1501/CS1501-Assignments/Assignment3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{434884D2-0C72-3449-9706-C23A4BAF6236}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3BD0E5-7881-9E47-83F9-09B3DC365F22}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="460" windowWidth="24860" windowHeight="20540" xr2:uid="{E6B10C25-E466-8242-B42A-DC14DF1F8046}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="33320" windowHeight="20540" xr2:uid="{E6B10C25-E466-8242-B42A-DC14DF1F8046}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -112,10 +112,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="0.000"/>
-    <numFmt numFmtId="175" formatCode="#,##0.000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -161,13 +157,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -185,33 +208,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="#,##0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
       <font>
@@ -245,26 +241,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D04E984-9874-F045-A51F-3A5119896658}" name="Table1" displayName="Table1" ref="B2:K16" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D04E984-9874-F045-A51F-3A5119896658}" name="Table1" displayName="Table1" ref="B2:K16" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="B2:K16" xr:uid="{EBE0CAED-E985-6E45-A6FD-8363D5671431}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D890BBDB-102C-9C40-BAD7-5C53FF91C427}" name="Column1" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{6ECF9DE6-F68F-AF44-9447-53A1C943F670}" name="Original" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{C444FC08-D9F8-A149-A999-CA1EAC2F77B1}" name="LZW" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{AA3F975C-8CE3-4B41-882C-80085F9B17A0}" name="LZW C.R." dataDxfId="7">
-      <calculatedColumnFormula>D3/C3</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{D890BBDB-102C-9C40-BAD7-5C53FF91C427}" name="Column1" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6ECF9DE6-F68F-AF44-9447-53A1C943F670}" name="Original" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{C444FC08-D9F8-A149-A999-CA1EAC2F77B1}" name="LZW" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{AA3F975C-8CE3-4B41-882C-80085F9B17A0}" name="LZW C.R." dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CABBFB55-AA03-084B-956E-59B48480BE7E}" name="LZWmod (no reset)" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{293DFD7E-0BE8-0D43-B703-FE78177D6C22}" name="LZWmod C.R." dataDxfId="5">
-      <calculatedColumnFormula>F3/C3</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{CABBFB55-AA03-084B-956E-59B48480BE7E}" name="LZWmod (no reset)" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{293DFD7E-0BE8-0D43-B703-FE78177D6C22}" name="LZWmod C.R." dataDxfId="3">
+      <calculatedColumnFormula>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{651F0A88-8CF9-C240-B4E3-D601CAD8078D}" name="LZWmod (with reset)" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{5AFCABA5-B075-7649-B487-F70B6B616087}" name="LZWmod(R) C.R." dataDxfId="3">
-      <calculatedColumnFormula>H3/C3</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{5AFCABA5-B075-7649-B487-F70B6B616087}" name="LZWmod(R) C.R." dataDxfId="5">
+      <calculatedColumnFormula>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4B579B2C-6233-2F45-B2CB-EDB72D4E4488}" name="Unix Compress" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{314FE5AD-0A47-B440-96FC-3F02E206DF44}" name="Unix C.R." dataDxfId="1">
-      <calculatedColumnFormula>J3/C3</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{4B579B2C-6233-2F45-B2CB-EDB72D4E4488}" name="Unix Compress" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{314FE5AD-0A47-B440-96FC-3F02E206DF44}" name="Unix C.R." dataDxfId="7">
+      <calculatedColumnFormula>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -571,7 +567,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="K16" sqref="B2:K16"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,29 +641,29 @@
         <v>128973</v>
       </c>
       <c r="E3" s="5">
-        <f>D3/C3</f>
-        <v>1.3812961197802316</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>0.7239577275863941</v>
       </c>
       <c r="F3" s="1">
         <v>122493</v>
       </c>
       <c r="G3" s="5">
-        <f>F3/C3</f>
-        <v>1.3118955564361525</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>0.76225580237238044</v>
       </c>
       <c r="H3" s="1">
         <v>122493</v>
       </c>
       <c r="I3" s="6">
-        <f>H3/C3</f>
-        <v>1.3118955564361525</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>0.76225580237238044</v>
       </c>
       <c r="J3" s="1">
         <v>93213</v>
       </c>
       <c r="K3" s="5">
-        <f>J3/C3</f>
-        <v>0.99830782577031407</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>1.0016950425369853</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -682,29 +678,29 @@
         <v>1846854</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E16" si="0">D4/C4</f>
-        <v>0.60931363492398649</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>1.6411909116800787</v>
       </c>
       <c r="F4" s="1">
-        <v>1792783</v>
+        <v>1792781</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" ref="G4:G16" si="1">F4/C4</f>
-        <v>0.59147454339104732</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>1.6906917241983266</v>
       </c>
       <c r="H4" s="1">
-        <v>1249015</v>
+        <v>1177887</v>
       </c>
       <c r="I4" s="6">
-        <f t="shared" ref="I4:I16" si="2">H4/C4</f>
-        <v>0.41207473342483109</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>2.573285892449785</v>
       </c>
       <c r="J4" s="1">
         <v>1179467</v>
       </c>
       <c r="K4" s="5">
-        <f t="shared" ref="K4:K16" si="3">J4/C4</f>
-        <v>0.38912947371199325</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>2.5698387491977308</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -719,29 +715,29 @@
         <v>74574</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>0.85677849264705885</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>1.1671628181403706</v>
       </c>
       <c r="F5" s="1">
         <v>40040</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" si="1"/>
-        <v>0.46001838235294118</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>2.1738261738261739</v>
       </c>
       <c r="H5" s="2">
         <v>40040</v>
       </c>
       <c r="I5" s="6">
-        <f t="shared" si="2"/>
-        <v>0.46001838235294118</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>2.1738261738261739</v>
       </c>
       <c r="J5" s="1">
         <v>40040</v>
       </c>
       <c r="K5" s="5">
-        <f t="shared" si="3"/>
-        <v>0.46001838235294118</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>2.1738261738261739</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -756,29 +752,29 @@
         <v>925079</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>0.83647913049768519</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>1.1954870881297706</v>
       </c>
       <c r="F6" s="1">
         <v>80913</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="1"/>
-        <v>7.3163519965277785E-2</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>13.668013792592044</v>
       </c>
       <c r="H6" s="1">
         <v>80913</v>
       </c>
       <c r="I6" s="6">
-        <f t="shared" si="2"/>
-        <v>7.3163519965277785E-2</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>13.668013792592044</v>
       </c>
       <c r="J6" s="1">
         <v>80913</v>
       </c>
       <c r="K6" s="5">
-        <f t="shared" si="3"/>
-        <v>7.3163519965277785E-2</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>13.668013792592044</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -793,29 +789,29 @@
         <v>30980</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="0"/>
-        <v>0.42819034982239362</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>2.3354099418979986</v>
       </c>
       <c r="F7" s="1">
         <v>24544</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="1"/>
-        <v>0.33923511769014941</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>2.9478080182529336</v>
       </c>
       <c r="H7" s="1">
         <v>24544</v>
       </c>
       <c r="I7" s="6">
-        <f t="shared" si="2"/>
-        <v>0.33923511769014941</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>2.9478080182529336</v>
       </c>
       <c r="J7" s="1">
         <v>24545</v>
       </c>
       <c r="K7" s="5">
-        <f t="shared" si="3"/>
-        <v>0.33924893919918175</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>2.9476879201466692</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -830,29 +826,29 @@
         <v>24138</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="0"/>
-        <v>0.41832897176825357</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>2.3904631701052281</v>
       </c>
       <c r="F8" s="1">
         <v>20516</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="1"/>
-        <v>0.355557096064193</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>2.8124878143887697</v>
       </c>
       <c r="H8" s="1">
         <v>20516</v>
       </c>
       <c r="I8" s="6">
-        <f t="shared" si="2"/>
-        <v>0.355557096064193</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>2.8124878143887697</v>
       </c>
       <c r="J8" s="1">
         <v>20516</v>
       </c>
       <c r="K8" s="5">
-        <f t="shared" si="3"/>
-        <v>0.355557096064193</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>2.8124878143887697</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -867,29 +863,29 @@
         <v>250742</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>1.0609915033343489</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>0.94251461661787816</v>
       </c>
       <c r="F9" s="1">
-        <v>156411</v>
+        <v>156409</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="1"/>
-        <v>0.66183863105514373</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>1.5109616454296109</v>
       </c>
       <c r="H9" s="1">
-        <v>158297</v>
+        <v>152231</v>
       </c>
       <c r="I9" s="6">
-        <f t="shared" si="2"/>
-        <v>0.66981906502826583</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>1.5524301883322056</v>
       </c>
       <c r="J9" s="1">
         <v>151111</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" si="3"/>
-        <v>0.63941217291222374</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>1.5639364440709147</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -904,28 +900,28 @@
         <v>177453</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4000457600908891</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>0.71426236806365628</v>
       </c>
       <c r="F10" s="1">
         <v>163789</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" si="1"/>
-        <v>1.2922412976930602</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>0.7738492816977941</v>
       </c>
       <c r="H10" s="1">
-        <v>178499</v>
+        <v>171170</v>
       </c>
       <c r="I10" s="6">
-        <f t="shared" si="2"/>
-        <v>1.4082983557925963</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>0.74048022433837701</v>
       </c>
       <c r="J10" s="1">
         <v>126748</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" si="3"/>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
         <v>1</v>
       </c>
     </row>
@@ -941,29 +937,29 @@
         <v>9278</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="0"/>
-        <v>0.53518689432395017</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>1.8685061435654235</v>
       </c>
       <c r="F11" s="1">
         <v>8963</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="1"/>
-        <v>0.51701661282879552</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>1.9341738257279928</v>
       </c>
       <c r="H11" s="1">
         <v>8963</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" si="2"/>
-        <v>0.51701661282879552</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>1.9341738257279928</v>
       </c>
       <c r="J11" s="1">
         <v>8964</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="3"/>
-        <v>0.51707429626211354</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>1.9339580544399821</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -978,29 +974,29 @@
         <v>605184</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="0"/>
-        <v>0.49576678356651865</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>2.017077450824873</v>
       </c>
       <c r="F12" s="1">
-        <v>501779</v>
+        <v>501777</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="1"/>
-        <v>0.41105739889227766</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>2.4327599710628425</v>
       </c>
       <c r="H12" s="1">
-        <v>556867</v>
+        <v>527598</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="2"/>
-        <v>0.45618549311339451</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>2.3136990663345958</v>
       </c>
       <c r="J12" s="1">
         <v>522673</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="3"/>
-        <v>0.42817376544499358</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>2.3355003989109826</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1015,29 +1011,29 @@
         <v>13197</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="0"/>
-        <v>0.51942378084779783</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>1.9252102750625142</v>
       </c>
       <c r="F13" s="1">
         <v>12531</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49321053253040503</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>2.027531721331099</v>
       </c>
       <c r="H13" s="1">
         <v>12531</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="2"/>
-        <v>0.49321053253040503</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>2.027531721331099</v>
       </c>
       <c r="J13" s="1">
         <v>12531</v>
       </c>
       <c r="K13" s="5">
-        <f t="shared" si="3"/>
-        <v>0.49321053253040503</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>2.027531721331099</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1052,29 +1048,29 @@
         <v>1012179</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.73218967013888892</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>1.3657663318444662</v>
       </c>
       <c r="F14" s="1">
-        <v>597849</v>
+        <v>597847</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="1"/>
-        <v>0.43247178819444443</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>2.3122972934546797</v>
       </c>
       <c r="H14" s="1">
-        <v>622157</v>
+        <v>590545</v>
       </c>
       <c r="I14" s="6">
-        <f t="shared" si="2"/>
-        <v>0.4500557002314815</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>2.3408885012996468</v>
       </c>
       <c r="J14" s="1">
         <v>589697</v>
       </c>
       <c r="K14" s="5">
-        <f t="shared" si="3"/>
-        <v>0.42657479745370369</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>2.3442547613435374</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1089,29 +1085,29 @@
         <v>4302</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="0"/>
-        <v>4.6676952522313143E-3</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>214.23849372384936</v>
       </c>
       <c r="F15" s="1">
         <v>3951</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="1"/>
-        <v>4.2868581919028185E-3</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>233.27107061503418</v>
       </c>
       <c r="H15" s="1">
         <v>3951</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="2"/>
-        <v>4.2868581919028185E-3</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>233.27107061503418</v>
       </c>
       <c r="J15" s="1">
         <v>3952</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="3"/>
-        <v>4.2879431977726999E-3</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>233.21204453441297</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1126,29 +1122,29 @@
         <v>159050</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="0"/>
-        <v>1.0127734902320369</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZW]]</f>
+        <v>0.98738761395787489</v>
       </c>
       <c r="F16" s="1">
         <v>62931</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="1"/>
-        <v>0.40072209062428366</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (no reset)]]</f>
+        <v>2.4954950660246937</v>
       </c>
       <c r="H16" s="1">
         <v>62931</v>
       </c>
       <c r="I16" s="6">
-        <f t="shared" si="2"/>
-        <v>0.40072209062428366</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[LZWmod (with reset)]]</f>
+        <v>2.4954950660246937</v>
       </c>
       <c r="J16" s="1">
         <v>62931</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.40072209062428366</v>
+        <f>Table1[[#This Row],[Original]]/Table1[[#This Row],[Unix Compress]]</f>
+        <v>2.4954950660246937</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add initial files for assignment 4
</commit_message>
<xml_diff>
--- a/Assignment3/CompressionResults.xlsx
+++ b/Assignment3/CompressionResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewhrydil/Desktop/CurrentClassesLocal/CS1501/CS1501-Assignments/Assignment3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3BD0E5-7881-9E47-83F9-09B3DC365F22}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E9A109-11AB-E348-85FD-F4779633CB23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="33320" windowHeight="20540" xr2:uid="{E6B10C25-E466-8242-B42A-DC14DF1F8046}"/>
   </bookViews>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A6086E-FFE6-7A4E-BD3E-8058E061F7E9}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="K16" sqref="B2:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1153,6 +1153,7 @@
     <mergeCell ref="B1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>